<commit_message>
adding past inputs and outputs for the model
</commit_message>
<xml_diff>
--- a/inputs/catalog.xlsx
+++ b/inputs/catalog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimenofonseca/Documents/CoolingTower/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E2B34D-E9C7-5147-858D-D1662964FF31}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A573A0A4-6A2F-974E-931E-EFFCC8442897}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6380" yWindow="540" windowWidth="19140" windowHeight="14920" xr2:uid="{AC97869F-F1BD-A544-8322-5476B2CD55A7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>CT</t>
   </si>
@@ -78,13 +78,16 @@
     <t>approach [C°]</t>
   </si>
   <si>
-    <t>WBT [C°]</t>
-  </si>
-  <si>
     <t>HWT [°C]</t>
   </si>
   <si>
-    <t>CWT °C]</t>
+    <t>CWT [°C]</t>
+  </si>
+  <si>
+    <t>WBT [°C]</t>
+  </si>
+  <si>
+    <t>Fan area [m2]</t>
   </si>
 </sst>
 </file>
@@ -100,11 +103,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF008080"/>
-      <name val="Menlo"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -127,9 +130,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA1F13C-C5A6-0845-B39F-3E008148622C}">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -468,60 +472,63 @@
     <col min="17" max="17" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="J1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>100</v>
       </c>
@@ -535,38 +542,49 @@
         <v>32.799999999999997</v>
       </c>
       <c r="E2">
-        <v>29.730080000000001</v>
+        <v>29.7340082748869</v>
       </c>
       <c r="F2">
-        <v>3.0659920000000001</v>
+        <v>3.0659917251130802</v>
       </c>
       <c r="G2">
         <v>5.2</v>
       </c>
       <c r="H2">
-        <v>4.59</v>
+        <v>4.5962641564936</v>
       </c>
       <c r="I2">
-        <v>2.27</v>
+        <v>2.2772400961256798</v>
       </c>
       <c r="J2">
-        <v>2.02</v>
+        <v>2.0183485106877002</v>
       </c>
       <c r="K2">
-        <v>0.78</v>
+        <v>0.78223357474255195</v>
       </c>
       <c r="L2">
         <v>0.9</v>
       </c>
       <c r="M2">
-        <v>0.65</v>
+        <v>0.64773735458917103</v>
       </c>
       <c r="N2">
-        <v>13.5</v>
-      </c>
-      <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+        <v>13.540172138692199</v>
+      </c>
+      <c r="O2">
+        <v>4</v>
+      </c>
+      <c r="P2">
+        <v>1.2</v>
+      </c>
+      <c r="Q2">
+        <v>0.2</v>
+      </c>
+      <c r="R2">
+        <v>0.63617251235193295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>150</v>
       </c>
@@ -580,37 +598,49 @@
         <v>32.799999999999997</v>
       </c>
       <c r="E3">
-        <v>29.730080000000001</v>
+        <v>29.7340082748869</v>
       </c>
       <c r="F3">
-        <v>3.0659920000000001</v>
+        <v>3.0659917251130802</v>
       </c>
       <c r="G3">
         <v>5.2</v>
       </c>
       <c r="H3">
-        <v>6.89</v>
+        <v>6.8943962347404</v>
       </c>
       <c r="I3">
-        <v>3.41</v>
+        <v>3.4158601441885201</v>
       </c>
       <c r="J3">
-        <v>2.02</v>
+        <v>2.0183485106877002</v>
       </c>
       <c r="K3">
-        <v>0.78</v>
+        <v>0.78223357474255195</v>
       </c>
       <c r="L3">
         <v>0.9</v>
       </c>
       <c r="M3">
-        <v>0.65</v>
+        <v>0.64773735458917103</v>
       </c>
       <c r="N3">
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+        <v>13.540172138692199</v>
+      </c>
+      <c r="O3">
+        <v>4</v>
+      </c>
+      <c r="P3">
+        <v>1.2</v>
+      </c>
+      <c r="Q3">
+        <v>0.2</v>
+      </c>
+      <c r="R3">
+        <v>0.63617251235193295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>200</v>
       </c>
@@ -624,37 +654,49 @@
         <v>32.799999999999997</v>
       </c>
       <c r="E4">
-        <v>29.730080000000001</v>
+        <v>29.7340082748869</v>
       </c>
       <c r="F4">
-        <v>3.0659920000000001</v>
+        <v>3.0659917251130802</v>
       </c>
       <c r="G4">
         <v>5.2</v>
       </c>
       <c r="H4">
-        <v>9.19</v>
+        <v>9.1925283129872</v>
       </c>
       <c r="I4">
-        <v>4.55</v>
+        <v>4.5544801922513596</v>
       </c>
       <c r="J4">
-        <v>2.02</v>
+        <v>2.0183485106877002</v>
       </c>
       <c r="K4">
-        <v>0.78</v>
+        <v>0.78223357474255195</v>
       </c>
       <c r="L4">
         <v>1.2</v>
       </c>
       <c r="M4">
-        <v>0.65</v>
+        <v>0.64773735458917103</v>
       </c>
       <c r="N4">
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+        <v>13.540172138692199</v>
+      </c>
+      <c r="O4">
+        <v>4</v>
+      </c>
+      <c r="P4">
+        <v>1.2</v>
+      </c>
+      <c r="Q4">
+        <v>0.2</v>
+      </c>
+      <c r="R4">
+        <v>1.13097335529232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>300</v>
       </c>
@@ -668,37 +710,49 @@
         <v>32.799999999999997</v>
       </c>
       <c r="E5">
-        <v>29.730080000000001</v>
+        <v>29.7340082748869</v>
       </c>
       <c r="F5">
-        <v>3.0659920000000001</v>
+        <v>3.0659917251130802</v>
       </c>
       <c r="G5">
         <v>5.2</v>
       </c>
       <c r="H5">
-        <v>13.79</v>
+        <v>13.7887924694808</v>
       </c>
       <c r="I5">
-        <v>6.83</v>
+        <v>6.8317202883770403</v>
       </c>
       <c r="J5">
-        <v>2.02</v>
+        <v>2.0183485106877002</v>
       </c>
       <c r="K5">
-        <v>0.78</v>
+        <v>0.78223357474255195</v>
       </c>
       <c r="L5">
         <v>1.2</v>
       </c>
       <c r="M5">
-        <v>0.65</v>
+        <v>0.64773735458917103</v>
       </c>
       <c r="N5">
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+        <v>13.540172138692199</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
+      <c r="P5">
+        <v>1.2</v>
+      </c>
+      <c r="Q5">
+        <v>0.2</v>
+      </c>
+      <c r="R5">
+        <v>1.13097335529232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>400</v>
       </c>
@@ -712,37 +766,49 @@
         <v>32.799999999999997</v>
       </c>
       <c r="E6">
-        <v>29.730080000000001</v>
+        <v>29.7340082748869</v>
       </c>
       <c r="F6">
-        <v>3.0659920000000001</v>
+        <v>3.0659917251130802</v>
       </c>
       <c r="G6">
         <v>5.2</v>
       </c>
       <c r="H6">
-        <v>18.38</v>
+        <v>18.3850566259744</v>
       </c>
       <c r="I6">
-        <v>9.1</v>
+        <v>9.1089603845027192</v>
       </c>
       <c r="J6">
-        <v>2.02</v>
+        <v>2.0183485106877002</v>
       </c>
       <c r="K6">
-        <v>0.78</v>
+        <v>0.78223357474255195</v>
       </c>
       <c r="L6">
         <v>1.6</v>
       </c>
       <c r="M6">
-        <v>0.65</v>
+        <v>0.64773735458917103</v>
       </c>
       <c r="N6">
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+        <v>13.540172138692199</v>
+      </c>
+      <c r="O6">
+        <v>4</v>
+      </c>
+      <c r="P6">
+        <v>1.2</v>
+      </c>
+      <c r="Q6">
+        <v>0.2</v>
+      </c>
+      <c r="R6">
+        <v>2.0106192982974598</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>500</v>
       </c>
@@ -756,37 +822,49 @@
         <v>32.799999999999997</v>
       </c>
       <c r="E7">
-        <v>29.730080000000001</v>
+        <v>29.7340082748869</v>
       </c>
       <c r="F7">
-        <v>3.0659920000000001</v>
+        <v>3.0659917251130802</v>
       </c>
       <c r="G7">
         <v>5.2</v>
       </c>
       <c r="H7">
-        <v>22.98</v>
+        <v>22.981320782468</v>
       </c>
       <c r="I7">
-        <v>11.38</v>
+        <v>11.3862004806284</v>
       </c>
       <c r="J7">
-        <v>2.02</v>
+        <v>2.0183485106877002</v>
       </c>
       <c r="K7">
-        <v>0.78</v>
+        <v>0.78223357474255195</v>
       </c>
       <c r="L7">
         <v>1.6</v>
       </c>
       <c r="M7">
-        <v>0.65</v>
+        <v>0.64773735458917103</v>
       </c>
       <c r="N7">
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+        <v>13.540172138692199</v>
+      </c>
+      <c r="O7">
+        <v>4</v>
+      </c>
+      <c r="P7">
+        <v>1.2</v>
+      </c>
+      <c r="Q7">
+        <v>0.2</v>
+      </c>
+      <c r="R7">
+        <v>2.0106192982974598</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>800</v>
       </c>
@@ -800,34 +878,382 @@
         <v>32.799999999999997</v>
       </c>
       <c r="E8">
-        <v>29.730080000000001</v>
+        <v>29.7340082748869</v>
       </c>
       <c r="F8">
-        <v>3.0659920000000001</v>
+        <v>3.0659917251130802</v>
       </c>
       <c r="G8">
         <v>5.2</v>
       </c>
       <c r="H8">
-        <v>36.770000000000003</v>
+        <v>36.7701132519488</v>
       </c>
       <c r="I8">
-        <v>18.22</v>
+        <v>18.217920769005399</v>
       </c>
       <c r="J8">
-        <v>2.02</v>
+        <v>2.0183485106877002</v>
       </c>
       <c r="K8">
-        <v>0.78</v>
+        <v>0.78223357474255195</v>
       </c>
       <c r="L8">
         <v>2.2000000000000002</v>
       </c>
       <c r="M8">
-        <v>0.65</v>
+        <v>0.64773735458917103</v>
       </c>
       <c r="N8">
-        <v>13.5</v>
+        <v>13.540172138692199</v>
+      </c>
+      <c r="O8">
+        <v>4</v>
+      </c>
+      <c r="P8">
+        <v>1.2</v>
+      </c>
+      <c r="Q8">
+        <v>0.2</v>
+      </c>
+      <c r="R8">
+        <v>3.8013271108436499</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1000</v>
+      </c>
+      <c r="B9">
+        <v>1000</v>
+      </c>
+      <c r="C9">
+        <v>38</v>
+      </c>
+      <c r="D9">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="E9">
+        <v>29.7340082748869</v>
+      </c>
+      <c r="F9">
+        <v>3.0659917251130802</v>
+      </c>
+      <c r="G9">
+        <v>5.2</v>
+      </c>
+      <c r="H9">
+        <v>45.962641564936</v>
+      </c>
+      <c r="I9">
+        <v>22.7724009612568</v>
+      </c>
+      <c r="J9">
+        <v>2.0183485106877002</v>
+      </c>
+      <c r="K9">
+        <v>0.78223357474255195</v>
+      </c>
+      <c r="L9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M9">
+        <v>0.64773735458917103</v>
+      </c>
+      <c r="N9">
+        <v>13.540172138692199</v>
+      </c>
+      <c r="O9">
+        <v>4</v>
+      </c>
+      <c r="P9">
+        <v>1.2</v>
+      </c>
+      <c r="Q9">
+        <v>0.2</v>
+      </c>
+      <c r="R9">
+        <v>3.8013271108436499</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1700</v>
+      </c>
+      <c r="B10">
+        <v>1700</v>
+      </c>
+      <c r="C10">
+        <v>38</v>
+      </c>
+      <c r="D10">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="E10">
+        <v>29.7340082748869</v>
+      </c>
+      <c r="F10">
+        <v>3.0659917251130802</v>
+      </c>
+      <c r="G10">
+        <v>5.2</v>
+      </c>
+      <c r="H10">
+        <v>78.136490660391203</v>
+      </c>
+      <c r="I10">
+        <v>38.7130816341365</v>
+      </c>
+      <c r="J10">
+        <v>2.0183485106877002</v>
+      </c>
+      <c r="K10">
+        <v>0.78223357474255195</v>
+      </c>
+      <c r="L10">
+        <v>3.4</v>
+      </c>
+      <c r="M10">
+        <v>0.64773735458917103</v>
+      </c>
+      <c r="N10">
+        <v>13.540172138692199</v>
+      </c>
+      <c r="O10">
+        <v>4</v>
+      </c>
+      <c r="P10">
+        <v>1.2</v>
+      </c>
+      <c r="Q10">
+        <v>0.2</v>
+      </c>
+      <c r="R10">
+        <v>9.0792027688745005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2500</v>
+      </c>
+      <c r="B11">
+        <v>2500</v>
+      </c>
+      <c r="C11">
+        <v>38</v>
+      </c>
+      <c r="D11">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="E11">
+        <v>29.7340082748869</v>
+      </c>
+      <c r="F11">
+        <v>3.0659917251130802</v>
+      </c>
+      <c r="G11">
+        <v>5.2</v>
+      </c>
+      <c r="H11">
+        <v>114.90660391233899</v>
+      </c>
+      <c r="I11">
+        <v>56.931002403142003</v>
+      </c>
+      <c r="J11">
+        <v>2.0183485106877002</v>
+      </c>
+      <c r="K11">
+        <v>0.78223357474255195</v>
+      </c>
+      <c r="L11">
+        <v>3.4</v>
+      </c>
+      <c r="M11">
+        <v>0.64773735458917103</v>
+      </c>
+      <c r="N11">
+        <v>13.540172138692199</v>
+      </c>
+      <c r="O11">
+        <v>4</v>
+      </c>
+      <c r="P11">
+        <v>1.2</v>
+      </c>
+      <c r="Q11">
+        <v>0.2</v>
+      </c>
+      <c r="R11">
+        <v>9.0792027688745005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>5000</v>
+      </c>
+      <c r="B12">
+        <v>5000</v>
+      </c>
+      <c r="C12">
+        <v>38</v>
+      </c>
+      <c r="D12">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="E12">
+        <v>29.7340082748869</v>
+      </c>
+      <c r="F12">
+        <v>3.0659917251130802</v>
+      </c>
+      <c r="G12">
+        <v>5.2</v>
+      </c>
+      <c r="H12">
+        <v>229.81320782467901</v>
+      </c>
+      <c r="I12">
+        <v>113.86200480628401</v>
+      </c>
+      <c r="J12">
+        <v>2.0183485106877002</v>
+      </c>
+      <c r="K12">
+        <v>0.78223357474255195</v>
+      </c>
+      <c r="L12">
+        <v>4.8</v>
+      </c>
+      <c r="M12">
+        <v>0.64773735458917103</v>
+      </c>
+      <c r="N12">
+        <v>13.540172138692199</v>
+      </c>
+      <c r="O12">
+        <v>4</v>
+      </c>
+      <c r="P12">
+        <v>1.2</v>
+      </c>
+      <c r="Q12">
+        <v>0.2</v>
+      </c>
+      <c r="R12">
+        <v>18.095573684677198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>10000</v>
+      </c>
+      <c r="B13">
+        <v>10000</v>
+      </c>
+      <c r="C13">
+        <v>38</v>
+      </c>
+      <c r="D13">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="E13">
+        <v>29.7340082748869</v>
+      </c>
+      <c r="F13">
+        <v>3.0659917251130802</v>
+      </c>
+      <c r="G13">
+        <v>5.2</v>
+      </c>
+      <c r="H13">
+        <v>459.62641564935899</v>
+      </c>
+      <c r="I13">
+        <v>227.72400961256801</v>
+      </c>
+      <c r="J13">
+        <v>2.0183485106877002</v>
+      </c>
+      <c r="K13">
+        <v>0.78223357474255195</v>
+      </c>
+      <c r="L13">
+        <v>6.58</v>
+      </c>
+      <c r="M13">
+        <v>0.64773735458917103</v>
+      </c>
+      <c r="N13">
+        <v>13.540172138692199</v>
+      </c>
+      <c r="O13">
+        <v>4</v>
+      </c>
+      <c r="P13">
+        <v>1.2</v>
+      </c>
+      <c r="Q13">
+        <v>0.2</v>
+      </c>
+      <c r="R13">
+        <v>34.004913041721203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>50000</v>
+      </c>
+      <c r="B14">
+        <v>50000</v>
+      </c>
+      <c r="C14">
+        <v>38</v>
+      </c>
+      <c r="D14">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="E14">
+        <v>29.7340082748869</v>
+      </c>
+      <c r="F14">
+        <v>3.0659917251130802</v>
+      </c>
+      <c r="G14">
+        <v>5.2</v>
+      </c>
+      <c r="H14">
+        <v>2298.1320782468001</v>
+      </c>
+      <c r="I14">
+        <v>1138.6200480628399</v>
+      </c>
+      <c r="J14">
+        <v>2.0183485106877002</v>
+      </c>
+      <c r="K14">
+        <v>0.78223357474255195</v>
+      </c>
+      <c r="L14">
+        <v>15.59</v>
+      </c>
+      <c r="M14">
+        <v>0.64773735458917103</v>
+      </c>
+      <c r="N14">
+        <v>13.540172138692199</v>
+      </c>
+      <c r="O14">
+        <v>4</v>
+      </c>
+      <c r="P14">
+        <v>1.2</v>
+      </c>
+      <c r="Q14">
+        <v>0.2</v>
+      </c>
+      <c r="R14">
+        <v>190.88953135723901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>